<commit_message>
Convert to .csv and remove headers
</commit_message>
<xml_diff>
--- a/RoundBar_Options.xlsx
+++ b/RoundBar_Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schimmer\OneDrive - Rose-Hulman Institute of Technology\Documents\!! RHIT Fall 2021-22\EM204\EM204_Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22B0CBA5-1C10-4607-9F09-F7C5D14805A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34EC4E3-8594-4F9C-AE6B-B4781E56C03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1212" yWindow="1212" windowWidth="17280" windowHeight="9060" xr2:uid="{22413940-C5CD-4F9D-9A60-2322222B8B08}"/>
+    <workbookView xWindow="1515" yWindow="1575" windowWidth="21600" windowHeight="11325" xr2:uid="{22413940-C5CD-4F9D-9A60-2322222B8B08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,25 +34,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>OD</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -80,9 +68,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,356 +384,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F1CFBA-3E7F-40B2-B13D-DE8A72AEF3A9}">
-  <dimension ref="A1:A69"/>
+  <dimension ref="A1:A68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1">
+        <v>0.1875</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.1875</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.25</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.3125</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.375</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.4375</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.5</v>
+        <v>0.5625</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.5625</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0.625</v>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.6875</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0.75</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.8125</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0.875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>1.125</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1.125</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1.25</v>
+        <v>1.3125</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1.3125</v>
+        <v>1.375</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1.375</v>
+        <v>1.4375</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1.4375</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1.5</v>
+        <v>1.625</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1.625</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1.75</v>
+        <v>1.875</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1.875</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2</v>
+        <v>2.125</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2.125</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2.25</v>
+        <v>2.375</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2.375</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2.5</v>
+        <v>2.625</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2.625</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2.75</v>
+        <v>2.875</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2.875</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>3</v>
+        <v>3.125</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>3.125</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>3.25</v>
+        <v>3.375</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>3.375</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>3.5</v>
+        <v>3.625</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>3.625</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>3.75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>4</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>4.25</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>4.75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>5</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>5.25</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>5.75</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>6.5</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>6.75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>7</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>7.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>8.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>9</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>9.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>10</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>10.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>11</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>11.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>12</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>12.5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69">
         <v>21</v>
       </c>
     </row>

</xml_diff>